<commit_message>
Update cover in SubRES
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_IND_CCS_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_IND_CCS_Trans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF7F723-FC0B-44D4-9236-6404EE669F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5569FC88-E4CC-4303-9FC5-C69191E07EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="909" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="909" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="47" r:id="rId1"/>
@@ -19,7 +19,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
@@ -371,27 +370,15 @@
     <t>Document type:</t>
   </si>
   <si>
-    <t>Template type</t>
-  </si>
-  <si>
     <t>Sector(s):</t>
   </si>
   <si>
-    <t>Sector name</t>
-  </si>
-  <si>
     <t>Purpose:</t>
   </si>
   <si>
-    <t>Brief description of what this file is for</t>
-  </si>
-  <si>
     <t>Original developer(s):</t>
   </si>
   <si>
-    <t>Full Name(s) (Affiliation, email)</t>
-  </si>
-  <si>
     <t>Current maintainer(s):</t>
   </si>
   <si>
@@ -411,6 +398,18 @@
   </si>
   <si>
     <t>https://creativecommons.org/licenses/by-nc-sa/4.0/</t>
+  </si>
+  <si>
+    <t>New Technologies - Transformation</t>
+  </si>
+  <si>
+    <t>Specify regional availability of technologies</t>
+  </si>
+  <si>
+    <t>Olexandr Balyk (UCC, olexandr.balyk@ucc.ie)</t>
+  </si>
+  <si>
+    <t>Industry sector (IND)</t>
   </si>
 </sst>
 </file>
@@ -699,9 +698,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -720,9 +716,6 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -735,14 +728,20 @@
     <xf numFmtId="164" fontId="12" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1105,7 +1104,7 @@
                   <a14:compatExt spid="_x0000_s89089"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000015C0100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000015C0100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1273,19 +1272,6 @@
       <sheetData sheetId="56"/>
       <sheetData sheetId="57"/>
       <sheetData sheetId="58"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1615,8 +1601,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2054,20 +2040,20 @@
       <c r="Z15" s="16"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
       <c r="O16" s="16"/>
@@ -2084,10 +2070,10 @@
       <c r="Z16" s="16"/>
     </row>
     <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -2112,18 +2098,18 @@
       <c r="Z17" s="16"/>
     </row>
     <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
       <c r="M18" s="16"/>
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
@@ -2140,22 +2126,22 @@
       <c r="Z18" s="16"/>
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
+      <c r="B19" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
@@ -2172,22 +2158,22 @@
       <c r="Z19" s="16"/>
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
+      <c r="A20" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
       <c r="M20" s="16"/>
       <c r="N20" s="16"/>
       <c r="O20" s="16"/>
@@ -2204,22 +2190,22 @@
       <c r="Z20" s="16"/>
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
+      <c r="A21" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
       <c r="O21" s="16"/>
@@ -2236,18 +2222,18 @@
       <c r="Z21" s="16"/>
     </row>
     <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
       <c r="M22" s="16"/>
       <c r="N22" s="16"/>
       <c r="O22" s="16"/>
@@ -2264,14 +2250,14 @@
       <c r="Z22" s="16"/>
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
+      <c r="A23" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
@@ -2296,10 +2282,10 @@
       <c r="Z23" s="16"/>
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
@@ -2324,10 +2310,10 @@
       <c r="Z24" s="16"/>
     </row>
     <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
@@ -2352,14 +2338,14 @@
       <c r="Z25" s="16"/>
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
+      <c r="A26" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
@@ -2384,10 +2370,10 @@
       <c r="Z26" s="16"/>
     </row>
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
@@ -2412,10 +2398,10 @@
       <c r="Z27" s="16"/>
     </row>
     <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
@@ -2440,14 +2426,14 @@
       <c r="Z28" s="16"/>
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="29">
+      <c r="A29" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="27">
         <v>1</v>
       </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
@@ -2472,16 +2458,16 @@
       <c r="Z29" s="16"/>
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
+      <c r="A30" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
       <c r="G30" s="16"/>
       <c r="H30" s="16"/>
       <c r="I30" s="16"/>
@@ -2504,16 +2490,16 @@
       <c r="Z30" s="16"/>
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
+      <c r="A31" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
       <c r="I31" s="16"/>
@@ -2536,12 +2522,12 @@
       <c r="Z31" s="16"/>
     </row>
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
-      <c r="B32" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>

</xml_diff>